<commit_message>
updated BugTrackingsheet, fixed pagination padding
</commit_message>
<xml_diff>
--- a/BugTrackingSheet.xlsx
+++ b/BugTrackingSheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>Date Discovered</t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t>example bug</t>
+  </si>
+  <si>
+    <t>[Html] Footer won't stay down</t>
   </si>
 </sst>
 </file>
@@ -364,10 +367,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -411,6 +414,23 @@
         <v>5</v>
       </c>
     </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>42263.895833333336</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="2">
+        <v>42263</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added bug of duplicate names
Added the bug of duplicate names that is present within the QS text
scraper, hopefully will be able to fix tomorrow
</commit_message>
<xml_diff>
--- a/BugTrackingSheet.xlsx
+++ b/BugTrackingSheet.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh\Dropbox\UNI\2015\Sem 2\CITS3200\Webdev Work\unit-matching\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt\Documents\GitHub\unit-matching\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="15465" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="470" windowWidth="25610" windowHeight="15470" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>Date Discovered</t>
   </si>
@@ -60,6 +60,15 @@
   </si>
   <si>
     <t>Web management portal</t>
+  </si>
+  <si>
+    <t>QS text scraper features duplicate names</t>
+  </si>
+  <si>
+    <t>Matt</t>
+  </si>
+  <si>
+    <t>Ranking Scrape</t>
   </si>
 </sst>
 </file>
@@ -379,22 +388,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.875" customWidth="1"/>
-    <col min="2" max="2" width="33.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.375" customWidth="1"/>
-    <col min="5" max="5" width="21.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.58203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -410,7 +419,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>42261.354166666664</v>
       </c>
@@ -427,7 +436,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>42263.895833333336</v>
       </c>
@@ -444,8 +453,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
         <v>42277</v>
       </c>
       <c r="B4" t="s">
@@ -456,9 +465,24 @@
       </c>
       <c r="E4" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>42277.71875</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed duplicate name bug
Fixed the duplicate name bug in the text scraper. Couldn't work out how
to interface with database in time. Updated bug tracking sheet as well
</commit_message>
<xml_diff>
--- a/BugTrackingSheet.xlsx
+++ b/BugTrackingSheet.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\unit-matching\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt\Documents\GitHub\unit-matching\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="15465" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="470" windowWidth="25610" windowHeight="15470" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="21">
   <si>
     <t>Date Discovered</t>
   </si>
@@ -72,9 +72,6 @@
   </si>
   <si>
     <t>enter key does not submit form</t>
-  </si>
-  <si>
-    <t>josh</t>
   </si>
   <si>
     <t>web app</t>
@@ -412,18 +409,18 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="34.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.375" customWidth="1"/>
-    <col min="6" max="6" width="21.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.58203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="34.58203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" customWidth="1"/>
+    <col min="6" max="6" width="21.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -434,7 +431,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -443,7 +440,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>42261.354166666664</v>
       </c>
@@ -463,7 +460,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>42263.895833333336</v>
       </c>
@@ -483,7 +480,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>42277</v>
       </c>
@@ -500,7 +497,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>42277.71875</v>
       </c>
@@ -513,11 +510,14 @@
       <c r="D5" t="s">
         <v>13</v>
       </c>
+      <c r="E5" s="2">
+        <v>42285</v>
+      </c>
       <c r="F5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>42277</v>
       </c>
@@ -525,73 +525,73 @@
         <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E6" s="2">
         <v>42279</v>
       </c>
       <c r="F6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>42279</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E7" s="2">
         <v>42280</v>
       </c>
       <c r="F7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>42279</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" t="s">
         <v>16</v>
       </c>
-      <c r="D8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>42279</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E9" s="2">
         <v>42280</v>
       </c>
       <c r="F9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>